<commit_message>
change express-test value parsing and small fix
</commit_message>
<xml_diff>
--- a/backend/test.xlsx
+++ b/backend/test.xlsx
@@ -397,23 +397,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>modulation</v>
+        <v>Модуляция</v>
       </c>
       <c r="B1" t="str">
-        <v>bits</v>
+        <v>Аттен, ДБ</v>
       </c>
       <c r="C1" t="str">
-        <v>ebits</v>
+        <v>С/Ш</v>
       </c>
       <c r="D1" t="str">
-        <v>errorRate</v>
+        <v>Отправлено, байт</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Принято, байт</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Потерято, байт</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Процент ошибок, %</v>
       </c>
     </row>
     <row r="2">
@@ -421,18 +430,27 @@
         <v>QAM64 3/4</v>
       </c>
       <c r="B2">
-        <v>9593216</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="C2" t="str">
+        <v>26.350000381469727</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>16646272</v>
+      </c>
+      <c r="E2">
+        <v>16347840</v>
+      </c>
+      <c r="F2">
+        <v>298432</v>
+      </c>
+      <c r="G2">
+        <v>1.7927857961229996</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
integrated test duration in express-test
</commit_message>
<xml_diff>
--- a/backend/test.xlsx
+++ b/backend/test.xlsx
@@ -419,7 +419,7 @@
         <v>Принято, байт</v>
       </c>
       <c r="F1" t="str">
-        <v>Потерято, байт</v>
+        <v>Потеряно, байт</v>
       </c>
       <c r="G1" t="str">
         <v>Процент ошибок, %</v>
@@ -433,19 +433,19 @@
         <v>20</v>
       </c>
       <c r="C2" t="str">
-        <v>26.350000381469727</v>
+        <v>26.899999618530273</v>
       </c>
       <c r="D2">
-        <v>16646272</v>
+        <v>115416192</v>
       </c>
       <c r="E2">
-        <v>16347840</v>
+        <v>113735808</v>
       </c>
       <c r="F2">
-        <v>298432</v>
+        <v>1680384</v>
       </c>
       <c r="G2">
-        <v>1.7927857961229996</v>
+        <v>1.4559343631784352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some changes in express test logic
</commit_message>
<xml_diff>
--- a/backend/test.xlsx
+++ b/backend/test.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -436,27 +436,75 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>26.64</v>
+        <v>26.5</v>
       </c>
       <c r="D2">
-        <v>115476608</v>
+        <v>105416832</v>
       </c>
       <c r="E2">
-        <v>113791104</v>
+        <v>103889024</v>
       </c>
       <c r="F2">
-        <v>1685504</v>
+        <v>1527808</v>
       </c>
       <c r="G2">
-        <v>1.46</v>
+        <v>1.45</v>
       </c>
       <c r="H2" t="str">
         <v>Не пройдено</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>QAM64 2/3</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Ошибка поиска модуляции</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>QAM16 3/4</v>
+      </c>
+      <c r="H4" t="str">
+        <v>Ошибка поиска модуляции</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>QAM16 1/2</v>
+      </c>
+      <c r="H5" t="str">
+        <v>Ошибка поиска модуляции</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>QPSK 3/4</v>
+      </c>
+      <c r="H6" t="str">
+        <v>Ошибка поиска модуляции</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>QPSK 1/2</v>
+      </c>
+      <c r="H7" t="str">
+        <v>Ошибка поиска модуляции</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>BPSK 1/2</v>
+      </c>
+      <c r="H8" t="str">
+        <v>Ошибка поиска модуляции</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>